<commit_message>
add report pdf & slides
</commit_message>
<xml_diff>
--- a/Testcase Reports & Slides/Testcase_Report.xlsx
+++ b/Testcase Reports & Slides/Testcase_Report.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TAD\POMSelenium\Testcase Reports &amp; Slides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AC8D31-D853-44B2-9CB8-0BC40266AD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F06D60-82A4-4C1B-8436-BC033A4D4C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{30327C50-E0EB-4F96-A534-CCB957EA1EE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$23</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -834,10 +837,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF88E6CB-43F4-485D-A16A-D0FE2E3D76C2}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1292,7 @@
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A9:H10"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="96" fitToHeight="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>